<commit_message>
add tpc-ds tabel voor report
</commit_message>
<xml_diff>
--- a/10-tpc-ds/analysis/manual_comparative_result_analysis.xlsx
+++ b/10-tpc-ds/analysis/manual_comparative_result_analysis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorrit\Desktop\duckdb_bench\10-tpc-ds\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\various\duckdb_bench\10-tpc-ds\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19944" windowHeight="7728" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19944" windowHeight="7728" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="pg" sheetId="1" r:id="rId1"/>
@@ -17,16 +17,17 @@
     <sheet name="sbs_data" sheetId="2" r:id="rId3"/>
     <sheet name="sbs_pivot" sheetId="4" r:id="rId4"/>
     <sheet name="ratio_pivot" sheetId="5" r:id="rId5"/>
+    <sheet name="report_appendix_table" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="165">
   <si>
     <t>timestamp</t>
   </si>
@@ -510,11 +511,28 @@
   <si>
     <t>speedup ratio</t>
   </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Postgres
+[s]</t>
+  </si>
+  <si>
+    <t>DuckDB
+[s]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -651,7 +669,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -831,8 +849,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -947,6 +971,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -992,13 +1031,30 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6532,520 +6588,613 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>sbs_pivot!$A$5:$A$89</c:f>
+              <c:f>sbs_pivot!$A$5:$A$105</c:f>
               <c:strCache>
-                <c:ptCount val="84"/>
+                <c:ptCount val="100"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="18">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="19">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="20">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="21">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="22">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="23">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="26">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="27">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="28">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="31">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="32">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="33">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="36">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="37">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="38">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="39">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="40">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="41">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="42">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="43">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="44">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="45">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="46">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="47">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="48">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="49">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="50">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="51">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="52">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="55">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="56">
                   <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="57">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="58">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="59">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="60">
                   <c:v>61</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="61">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="62">
                   <c:v>63</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="63">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="64">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="65">
                   <c:v>66</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="66">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="67">
                   <c:v>68</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="68">
                   <c:v>69</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="69">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="70">
                   <c:v>71</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="71">
                   <c:v>72</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="72">
                   <c:v>73</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="75">
                   <c:v>76</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="76">
                   <c:v>77</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="77">
                   <c:v>78</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="78">
                   <c:v>79</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="79">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
                   <c:v>82</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="82">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="83">
                   <c:v>84</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="84">
                   <c:v>85</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="85">
                   <c:v>86</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="86">
                   <c:v>87</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="87">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="88">
                   <c:v>89</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="89">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="90">
                   <c:v>91</c:v>
                 </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="91">
                   <c:v>92</c:v>
                 </c:pt>
-                <c:pt idx="79">
+                <c:pt idx="92">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="80">
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
                   <c:v>96</c:v>
                 </c:pt>
-                <c:pt idx="81">
+                <c:pt idx="96">
                   <c:v>97</c:v>
                 </c:pt>
-                <c:pt idx="82">
+                <c:pt idx="97">
                   <c:v>98</c:v>
                 </c:pt>
-                <c:pt idx="83">
+                <c:pt idx="98">
                   <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>(blank)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sbs_pivot!$B$5:$B$89</c:f>
+              <c:f>sbs_pivot!$B$5:$B$105</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="84"/>
+                <c:ptCount val="100"/>
                 <c:pt idx="0">
+                  <c:v>360.01800036430302</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3.7479987144470202</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>6.8910002708434996</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>360.01500058174099</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>4.9449999332427899</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>360.01100015640202</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>4.1749997138976997</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>1.3580005168914699</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>13.4009993076324</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>64.7129998207092</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
+                  <c:v>360.01500129699701</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0.53599858283996504</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>3.0560004711151101</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
+                  <c:v>360.00499892234802</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>1.1760003566741899</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="15">
+                  <c:v>360.00399971008301</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>360.01799988746598</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>4.0940003395080504</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="18">
                   <c:v>3.2709991931915199</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="19">
                   <c:v>2.2240002155303902</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="20">
                   <c:v>10.644999980926499</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="21">
                   <c:v>158.01899957656801</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="22">
                   <c:v>156.75899815559299</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="23">
                   <c:v>5.4300007820129297</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="24">
+                  <c:v>360.01499843597401</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>4.0800004005432102</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="26">
                   <c:v>4.6739976406097403</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="27">
                   <c:v>28.235001087188699</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="28">
                   <c:v>11.0999996662139</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="29">
+                  <c:v>360.00699996948202</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>43.010000705718902</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="31">
                   <c:v>250.40202474594099</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="32">
                   <c:v>6.7539994716644198</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="33">
                   <c:v>4.2319991588592503</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="34">
+                  <c:v>360.01000022888098</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>8.7909998893737793</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="36">
                   <c:v>18.749999046325598</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="37">
                   <c:v>45.683999538421602</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="38">
                   <c:v>108.573999881744</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="39">
                   <c:v>3.12099981307983</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="40">
                   <c:v>33.771999835968003</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="41">
                   <c:v>4.28199911117553</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="42">
                   <c:v>8.4480009078979492</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="43">
                   <c:v>16.201998472213699</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="44">
                   <c:v>1.50599932670593</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="45">
                   <c:v>6.0770001411437899</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="46">
                   <c:v>58.686999082565301</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="47">
                   <c:v>12.483999490737901</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="48">
                   <c:v>17.402998208999598</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="49">
                   <c:v>8.0669999122619593</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="50">
                   <c:v>33.3270003795623</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="51">
                   <c:v>3.8679993152618399</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="52">
                   <c:v>4.7180001735687203</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="53">
+                  <c:v>360.01499962806702</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>3.91099905967712</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="55">
                   <c:v>8.6899998188018799</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="56">
                   <c:v>24.801000356674098</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="57">
                   <c:v>9.3379995822906494</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="58">
                   <c:v>37.342998027801499</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="59">
                   <c:v>8.75500035285949</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="60">
                   <c:v>7.9739995002746502</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="61">
                   <c:v>6.3209996223449698</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="62">
                   <c:v>4.44600057601928</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="63">
                   <c:v>18.912998676299999</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="64">
                   <c:v>26.490000009536701</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="65">
                   <c:v>5.9689984321594203</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="66">
                   <c:v>85.954000473022404</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="67">
                   <c:v>4.0339996814727703</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="68">
                   <c:v>17.325000047683702</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="69">
                   <c:v>22.0539999008178</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="70">
                   <c:v>7.3510003089904696</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="71">
                   <c:v>44.3009994029998</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="72">
                   <c:v>3.8640003204345699</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="73">
+                  <c:v>360.00800037383999</c:v>
+                </c:pt>
+                <c:pt idx="74">
                   <c:v>28.367000579833899</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="75">
                   <c:v>9.8130009174346906</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="76">
                   <c:v>9.2119987010955793</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="77">
                   <c:v>26.832000255584699</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="78">
                   <c:v>4.8450002670287997</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="79">
                   <c:v>11.4260003566741</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="80">
+                  <c:v>360.01600003242402</c:v>
+                </c:pt>
+                <c:pt idx="81">
                   <c:v>19.375999450683501</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="82">
                   <c:v>1.16900038719177</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="83">
                   <c:v>0.92900013923644997</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="84">
                   <c:v>5.1230006217956499</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="85">
                   <c:v>4.7509996891021702</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="86">
                   <c:v>47.340000391006399</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="87">
                   <c:v>32.6019992828369</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="88">
                   <c:v>6.4560000896453804</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="89">
                   <c:v>2.8880014419555602</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="90">
                   <c:v>0.73499846458435003</c:v>
                 </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="91">
                   <c:v>148.50999927520701</c:v>
                 </c:pt>
-                <c:pt idx="79">
+                <c:pt idx="92">
                   <c:v>7.95900130271911</c:v>
                 </c:pt>
-                <c:pt idx="80">
+                <c:pt idx="93">
+                  <c:v>360.00699996948202</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>360.01399993896399</c:v>
+                </c:pt>
+                <c:pt idx="95">
                   <c:v>4.5410003662109304</c:v>
                 </c:pt>
-                <c:pt idx="81">
+                <c:pt idx="96">
                   <c:v>14.308999538421601</c:v>
                 </c:pt>
-                <c:pt idx="82">
+                <c:pt idx="97">
                   <c:v>5.2159998416900599</c:v>
                 </c:pt>
-                <c:pt idx="83">
+                <c:pt idx="98">
                   <c:v>14.206000328063899</c:v>
                 </c:pt>
               </c:numCache>
@@ -7083,520 +7232,613 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>sbs_pivot!$A$5:$A$89</c:f>
+              <c:f>sbs_pivot!$A$5:$A$105</c:f>
               <c:strCache>
-                <c:ptCount val="84"/>
+                <c:ptCount val="100"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="18">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="19">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="20">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="21">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="22">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="23">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="26">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="27">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="28">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="31">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="32">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="33">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="36">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="37">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="38">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="39">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="40">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="41">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="42">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="43">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="44">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="45">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="46">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="47">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="48">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="49">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="50">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="51">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="52">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="55">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="56">
                   <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="57">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="58">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="59">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="60">
                   <c:v>61</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="61">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="62">
                   <c:v>63</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="63">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="64">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="65">
                   <c:v>66</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="66">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="67">
                   <c:v>68</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="68">
                   <c:v>69</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="69">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="70">
                   <c:v>71</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="71">
                   <c:v>72</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="72">
                   <c:v>73</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="75">
                   <c:v>76</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="76">
                   <c:v>77</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="77">
                   <c:v>78</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="78">
                   <c:v>79</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="79">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
                   <c:v>82</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="82">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="83">
                   <c:v>84</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="84">
                   <c:v>85</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="85">
                   <c:v>86</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="86">
                   <c:v>87</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="87">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="88">
                   <c:v>89</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="89">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="90">
                   <c:v>91</c:v>
                 </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="91">
                   <c:v>92</c:v>
                 </c:pt>
-                <c:pt idx="79">
+                <c:pt idx="92">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="80">
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
                   <c:v>96</c:v>
                 </c:pt>
-                <c:pt idx="81">
+                <c:pt idx="96">
                   <c:v>97</c:v>
                 </c:pt>
-                <c:pt idx="82">
+                <c:pt idx="97">
                   <c:v>98</c:v>
                 </c:pt>
-                <c:pt idx="83">
+                <c:pt idx="98">
                   <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>(blank)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sbs_pivot!$C$5:$C$89</c:f>
+              <c:f>sbs_pivot!$C$5:$C$105</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="84"/>
+                <c:ptCount val="100"/>
                 <c:pt idx="0">
+                  <c:v>9.6998691558837793E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.14099931716918901</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>8.2010269165038993E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>1.58899998664855</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.201006174087524</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>0.16199874877929599</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.117001056671142</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>6.6998958587646401E-2</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>0.36900067329406699</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>6.7000865936279297E-2</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
+                  <c:v>0.98100113868713301</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>4.2001962661743102E-2</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>0.122003316879272</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
+                  <c:v>1.3559980392455999</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>5.1999807357788003E-2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="15">
+                  <c:v>3.0999422073364199E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.8999977111816406E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0.189991950988769</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="18">
                   <c:v>7.3999404907226493E-2</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="19">
                   <c:v>5.2999973297119099E-2</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="20">
                   <c:v>3.7000179290771401E-2</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="21">
                   <c:v>1.8379993438720701</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="22">
                   <c:v>1.11200022697448</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="23">
                   <c:v>0.170999765396118</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="24">
+                  <c:v>7.6998233795166002E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>9.6001386642455999E-2</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="26">
                   <c:v>0.25000071525573703</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="27">
                   <c:v>0.29500198364257801</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="28">
                   <c:v>0.142001867294311</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="29">
+                  <c:v>0.12299990653991601</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>0.16199898719787501</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="31">
                   <c:v>1.0999917984008701E-2</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="32">
                   <c:v>7.3999404907226493E-2</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="33">
                   <c:v>0.10099983215331999</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="34">
+                  <c:v>0.304999589920043</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>0.25000166893005299</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="36">
                   <c:v>4.2999744415283203E-2</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="37">
                   <c:v>0.26200151443481401</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="38">
                   <c:v>0.279998779296875</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="39">
                   <c:v>5.5999755859375E-2</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="40">
                   <c:v>3.0999898910522398E-2</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="41">
                   <c:v>4.1000127792358398E-2</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="42">
                   <c:v>8.9000701904296806E-2</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="43">
                   <c:v>0.118000507354736</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="44">
                   <c:v>9.4999790191650293E-2</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="45">
                   <c:v>0.16799736022949199</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="46">
                   <c:v>0.52799963951110795</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="47">
                   <c:v>0.149005651473999</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="48">
                   <c:v>0.128981828689575</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="49">
                   <c:v>0.17499876022338801</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="50">
                   <c:v>2.0896501541137602</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="51">
                   <c:v>4.90002632141113E-2</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="52">
                   <c:v>7.7999591827392495E-2</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="53">
+                  <c:v>0.10300064086914</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>4.80005741119384E-2</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="55">
                   <c:v>0.111000299453735</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="56">
                   <c:v>0.35900020599365201</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="57">
                   <c:v>9.0001821517944294E-2</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="58">
                   <c:v>0.28899908065795898</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="59">
                   <c:v>0.12700200080871499</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="60">
                   <c:v>0.12499952316284101</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="61">
                   <c:v>6.3000440597534096E-2</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="62">
                   <c:v>6.9000244140625E-2</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="63">
                   <c:v>0.544999599456787</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="64">
                   <c:v>0.41500186920165999</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="65">
                   <c:v>0.183001518249511</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="66">
                   <c:v>4.0629978179931596</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="67">
                   <c:v>0.19999957084655701</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="68">
                   <c:v>0.14899849891662501</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="69">
                   <c:v>0.188999652862548</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="70">
                   <c:v>0.24599981307983301</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="71">
                   <c:v>0.41399908065795898</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="72">
                   <c:v>0.105998754501342</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="73">
+                  <c:v>0.84200024604797297</c:v>
+                </c:pt>
+                <c:pt idx="74">
                   <c:v>0.445999145507812</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="75">
                   <c:v>0.16200065612792899</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="76">
                   <c:v>9.3000173568725503E-2</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="77">
                   <c:v>1.85600090026855</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="78">
                   <c:v>0.18000054359435999</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="79">
                   <c:v>0.32800054550170898</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="80">
+                  <c:v>0.26199913024902299</c:v>
+                </c:pt>
+                <c:pt idx="81">
                   <c:v>8.0000877380371094E-2</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="82">
                   <c:v>8.8999748229980399E-2</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="83">
                   <c:v>9.9000692367553697E-2</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="84">
                   <c:v>0.124008178710937</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="85">
                   <c:v>0.120999097824096</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="86">
                   <c:v>0.37900972366333002</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="87">
                   <c:v>0.35899972915649397</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="88">
                   <c:v>0.164000034332275</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="89">
                   <c:v>2.6999473571777299E-2</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="90">
                   <c:v>3.5999298095703097E-2</c:v>
                 </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="91">
                   <c:v>4.6998977661132799E-2</c:v>
                 </c:pt>
-                <c:pt idx="79">
+                <c:pt idx="92">
                   <c:v>0.274999380111694</c:v>
                 </c:pt>
-                <c:pt idx="80">
+                <c:pt idx="93">
+                  <c:v>8.8999032974243095E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.72999811172485296</c:v>
+                </c:pt>
+                <c:pt idx="95">
                   <c:v>3.4998893737792899E-2</c:v>
                 </c:pt>
-                <c:pt idx="81">
+                <c:pt idx="96">
                   <c:v>0.38099908828735302</c:v>
                 </c:pt>
-                <c:pt idx="82">
+                <c:pt idx="97">
                   <c:v>0.49399995803833002</c:v>
                 </c:pt>
-                <c:pt idx="83">
+                <c:pt idx="98">
                   <c:v>9.8998308181762695E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -12274,7 +12516,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A4:C89" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <location ref="A4:C105" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" showAll="0">
       <items count="3">
@@ -12609,7 +12851,10 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="85">
+  <rowItems count="101">
+    <i>
+      <x/>
+    </i>
     <i>
       <x v="1"/>
     </i>
@@ -12617,7 +12862,13 @@
       <x v="2"/>
     </i>
     <i>
+      <x v="3"/>
+    </i>
+    <i>
       <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
     </i>
     <i>
       <x v="6"/>
@@ -12632,13 +12883,25 @@
       <x v="9"/>
     </i>
     <i>
+      <x v="10"/>
+    </i>
+    <i>
       <x v="11"/>
     </i>
     <i>
       <x v="12"/>
     </i>
     <i>
+      <x v="13"/>
+    </i>
+    <i>
       <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
     </i>
     <i>
       <x v="17"/>
@@ -12662,6 +12925,9 @@
       <x v="23"/>
     </i>
     <i>
+      <x v="24"/>
+    </i>
+    <i>
       <x v="25"/>
     </i>
     <i>
@@ -12674,6 +12940,9 @@
       <x v="28"/>
     </i>
     <i>
+      <x v="29"/>
+    </i>
+    <i>
       <x v="30"/>
     </i>
     <i>
@@ -12684,6 +12953,9 @@
     </i>
     <i>
       <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
     </i>
     <i>
       <x v="35"/>
@@ -12738,6 +13010,9 @@
     </i>
     <i>
       <x v="52"/>
+    </i>
+    <i>
+      <x v="53"/>
     </i>
     <i>
       <x v="54"/>
@@ -12797,6 +13072,9 @@
       <x v="72"/>
     </i>
     <i>
+      <x v="73"/>
+    </i>
+    <i>
       <x v="74"/>
     </i>
     <i>
@@ -12813,6 +13091,9 @@
     </i>
     <i>
       <x v="79"/>
+    </i>
+    <i>
+      <x v="80"/>
     </i>
     <i>
       <x v="81"/>
@@ -12851,6 +13132,12 @@
       <x v="92"/>
     </i>
     <i>
+      <x v="93"/>
+    </i>
+    <i>
+      <x v="94"/>
+    </i>
+    <i>
       <x v="95"/>
     </i>
     <i>
@@ -12861,6 +13148,9 @@
     </i>
     <i>
       <x v="98"/>
+    </i>
+    <i>
+      <x v="99"/>
     </i>
     <i t="grand">
       <x/>
@@ -12879,7 +13169,7 @@
   </colItems>
   <pageFields count="2">
     <pageField fld="0" hier="-1"/>
-    <pageField fld="5" item="0" hier="-1"/>
+    <pageField fld="5" hier="-1"/>
   </pageFields>
   <dataFields count="2">
     <dataField name="Sum of t_pg" fld="2" baseField="1" baseItem="0"/>
@@ -20092,10 +20382,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7:V7"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20122,8 +20412,8 @@
       <c r="A2" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="3">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -20139,937 +20429,1109 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>3.7479987144470202</v>
+        <v>360.01800036430302</v>
       </c>
       <c r="C5" s="2">
-        <v>0.14099931716918901</v>
+        <v>9.6998691558837793E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2">
-        <v>6.8910002708434996</v>
+        <v>3.7479987144470202</v>
       </c>
       <c r="C6" s="2">
-        <v>8.2010269165038993E-2</v>
+        <v>0.14099931716918901</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2">
-        <v>4.9449999332427899</v>
+        <v>6.8910002708434996</v>
       </c>
       <c r="C7" s="2">
-        <v>0.201006174087524</v>
+        <v>8.2010269165038993E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2">
-        <v>4.1749997138976997</v>
+        <v>360.01500058174099</v>
       </c>
       <c r="C8" s="2">
-        <v>0.117001056671142</v>
+        <v>1.58899998664855</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2">
-        <v>1.3580005168914699</v>
+        <v>4.9449999332427899</v>
       </c>
       <c r="C9" s="2">
-        <v>6.6998958587646401E-2</v>
+        <v>0.201006174087524</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2">
-        <v>13.4009993076324</v>
+        <v>360.01100015640202</v>
       </c>
       <c r="C10" s="2">
-        <v>0.36900067329406699</v>
+        <v>0.16199874877929599</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2">
-        <v>64.7129998207092</v>
+        <v>4.1749997138976997</v>
       </c>
       <c r="C11" s="2">
-        <v>6.7000865936279297E-2</v>
+        <v>0.117001056671142</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2">
-        <v>0.53599858283996504</v>
+        <v>1.3580005168914699</v>
       </c>
       <c r="C12" s="2">
-        <v>4.2001962661743102E-2</v>
+        <v>6.6998958587646401E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2">
-        <v>3.0560004711151101</v>
+        <v>13.4009993076324</v>
       </c>
       <c r="C13" s="2">
-        <v>0.122003316879272</v>
+        <v>0.36900067329406699</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2">
-        <v>1.1760003566741899</v>
+        <v>64.7129998207092</v>
       </c>
       <c r="C14" s="2">
-        <v>5.1999807357788003E-2</v>
+        <v>6.7000865936279297E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B15" s="2">
-        <v>4.0940003395080504</v>
+        <v>360.01500129699701</v>
       </c>
       <c r="C15" s="2">
-        <v>0.189991950988769</v>
+        <v>0.98100113868713301</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2">
-        <v>3.2709991931915199</v>
+        <v>0.53599858283996504</v>
       </c>
       <c r="C16" s="2">
-        <v>7.3999404907226493E-2</v>
+        <v>4.2001962661743102E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2">
-        <v>2.2240002155303902</v>
+        <v>3.0560004711151101</v>
       </c>
       <c r="C17" s="2">
-        <v>5.2999973297119099E-2</v>
+        <v>0.122003316879272</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2">
-        <v>10.644999980926499</v>
+        <v>360.00499892234802</v>
       </c>
       <c r="C18" s="2">
-        <v>3.7000179290771401E-2</v>
+        <v>1.3559980392455999</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2">
-        <v>158.01899957656801</v>
+        <v>1.1760003566741899</v>
       </c>
       <c r="C19" s="2">
-        <v>1.8379993438720701</v>
+        <v>5.1999807357788003E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2">
-        <v>156.75899815559299</v>
+        <v>360.00399971008301</v>
       </c>
       <c r="C20" s="2">
-        <v>1.11200022697448</v>
+        <v>3.0999422073364199E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B21" s="2">
-        <v>5.4300007820129297</v>
+        <v>360.01799988746598</v>
       </c>
       <c r="C21" s="2">
-        <v>0.170999765396118</v>
+        <v>9.8999977111816406E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B22" s="2">
-        <v>4.0800004005432102</v>
+        <v>4.0940003395080504</v>
       </c>
       <c r="C22" s="2">
-        <v>9.6001386642455999E-2</v>
+        <v>0.189991950988769</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B23" s="2">
-        <v>4.6739976406097403</v>
+        <v>3.2709991931915199</v>
       </c>
       <c r="C23" s="2">
-        <v>0.25000071525573703</v>
+        <v>7.3999404907226493E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B24" s="2">
-        <v>28.235001087188699</v>
+        <v>2.2240002155303902</v>
       </c>
       <c r="C24" s="2">
-        <v>0.29500198364257801</v>
+        <v>5.2999973297119099E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B25" s="2">
-        <v>11.0999996662139</v>
+        <v>10.644999980926499</v>
       </c>
       <c r="C25" s="2">
-        <v>0.142001867294311</v>
+        <v>3.7000179290771401E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B26" s="2">
-        <v>43.010000705718902</v>
+        <v>158.01899957656801</v>
       </c>
       <c r="C26" s="2">
-        <v>0.16199898719787501</v>
+        <v>1.8379993438720701</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B27" s="2">
-        <v>250.40202474594099</v>
+        <v>156.75899815559299</v>
       </c>
       <c r="C27" s="2">
-        <v>1.0999917984008701E-2</v>
+        <v>1.11200022697448</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B28" s="2">
-        <v>6.7539994716644198</v>
+        <v>5.4300007820129297</v>
       </c>
       <c r="C28" s="2">
-        <v>7.3999404907226493E-2</v>
+        <v>0.170999765396118</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B29" s="2">
-        <v>4.2319991588592503</v>
+        <v>360.01499843597401</v>
       </c>
       <c r="C29" s="2">
-        <v>0.10099983215331999</v>
+        <v>7.6998233795166002E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B30" s="2">
-        <v>8.7909998893737793</v>
+        <v>4.0800004005432102</v>
       </c>
       <c r="C30" s="2">
-        <v>0.25000166893005299</v>
+        <v>9.6001386642455999E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B31" s="2">
-        <v>18.749999046325598</v>
+        <v>4.6739976406097403</v>
       </c>
       <c r="C31" s="2">
-        <v>4.2999744415283203E-2</v>
+        <v>0.25000071525573703</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B32" s="2">
-        <v>45.683999538421602</v>
+        <v>28.235001087188699</v>
       </c>
       <c r="C32" s="2">
-        <v>0.26200151443481401</v>
+        <v>0.29500198364257801</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B33" s="2">
-        <v>108.573999881744</v>
+        <v>11.0999996662139</v>
       </c>
       <c r="C33" s="2">
-        <v>0.279998779296875</v>
+        <v>0.142001867294311</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B34" s="2">
-        <v>3.12099981307983</v>
+        <v>360.00699996948202</v>
       </c>
       <c r="C34" s="2">
-        <v>5.5999755859375E-2</v>
+        <v>0.12299990653991601</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B35" s="2">
-        <v>33.771999835968003</v>
+        <v>43.010000705718902</v>
       </c>
       <c r="C35" s="2">
-        <v>3.0999898910522398E-2</v>
+        <v>0.16199898719787501</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B36" s="2">
-        <v>4.28199911117553</v>
+        <v>250.40202474594099</v>
       </c>
       <c r="C36" s="2">
-        <v>4.1000127792358398E-2</v>
+        <v>1.0999917984008701E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B37" s="2">
-        <v>8.4480009078979492</v>
+        <v>6.7539994716644198</v>
       </c>
       <c r="C37" s="2">
-        <v>8.9000701904296806E-2</v>
+        <v>7.3999404907226493E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B38" s="2">
-        <v>16.201998472213699</v>
+        <v>4.2319991588592503</v>
       </c>
       <c r="C38" s="2">
-        <v>0.118000507354736</v>
+        <v>0.10099983215331999</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B39" s="2">
-        <v>1.50599932670593</v>
+        <v>360.01000022888098</v>
       </c>
       <c r="C39" s="2">
-        <v>9.4999790191650293E-2</v>
+        <v>0.304999589920043</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B40" s="2">
-        <v>6.0770001411437899</v>
+        <v>8.7909998893737793</v>
       </c>
       <c r="C40" s="2">
-        <v>0.16799736022949199</v>
+        <v>0.25000166893005299</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B41" s="2">
-        <v>58.686999082565301</v>
+        <v>18.749999046325598</v>
       </c>
       <c r="C41" s="2">
-        <v>0.52799963951110795</v>
+        <v>4.2999744415283203E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B42" s="2">
-        <v>12.483999490737901</v>
+        <v>45.683999538421602</v>
       </c>
       <c r="C42" s="2">
-        <v>0.149005651473999</v>
+        <v>0.26200151443481401</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B43" s="2">
-        <v>17.402998208999598</v>
+        <v>108.573999881744</v>
       </c>
       <c r="C43" s="2">
-        <v>0.128981828689575</v>
+        <v>0.279998779296875</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B44" s="2">
-        <v>8.0669999122619593</v>
+        <v>3.12099981307983</v>
       </c>
       <c r="C44" s="2">
-        <v>0.17499876022338801</v>
+        <v>5.5999755859375E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B45" s="2">
-        <v>33.3270003795623</v>
+        <v>33.771999835968003</v>
       </c>
       <c r="C45" s="2">
-        <v>2.0896501541137602</v>
+        <v>3.0999898910522398E-2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B46" s="2">
-        <v>3.8679993152618399</v>
+        <v>4.28199911117553</v>
       </c>
       <c r="C46" s="2">
-        <v>4.90002632141113E-2</v>
+        <v>4.1000127792358398E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B47" s="2">
-        <v>4.7180001735687203</v>
+        <v>8.4480009078979492</v>
       </c>
       <c r="C47" s="2">
-        <v>7.7999591827392495E-2</v>
+        <v>8.9000701904296806E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B48" s="2">
-        <v>3.91099905967712</v>
+        <v>16.201998472213699</v>
       </c>
       <c r="C48" s="2">
-        <v>4.80005741119384E-2</v>
+        <v>0.118000507354736</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B49" s="2">
-        <v>8.6899998188018799</v>
+        <v>1.50599932670593</v>
       </c>
       <c r="C49" s="2">
-        <v>0.111000299453735</v>
+        <v>9.4999790191650293E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B50" s="2">
-        <v>24.801000356674098</v>
+        <v>6.0770001411437899</v>
       </c>
       <c r="C50" s="2">
-        <v>0.35900020599365201</v>
+        <v>0.16799736022949199</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B51" s="2">
-        <v>9.3379995822906494</v>
+        <v>58.686999082565301</v>
       </c>
       <c r="C51" s="2">
-        <v>9.0001821517944294E-2</v>
+        <v>0.52799963951110795</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B52" s="2">
-        <v>37.342998027801499</v>
+        <v>12.483999490737901</v>
       </c>
       <c r="C52" s="2">
-        <v>0.28899908065795898</v>
+        <v>0.149005651473999</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B53" s="2">
-        <v>8.75500035285949</v>
+        <v>17.402998208999598</v>
       </c>
       <c r="C53" s="2">
-        <v>0.12700200080871499</v>
+        <v>0.128981828689575</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B54" s="2">
-        <v>7.9739995002746502</v>
+        <v>8.0669999122619593</v>
       </c>
       <c r="C54" s="2">
-        <v>0.12499952316284101</v>
+        <v>0.17499876022338801</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B55" s="2">
-        <v>6.3209996223449698</v>
+        <v>33.3270003795623</v>
       </c>
       <c r="C55" s="2">
-        <v>6.3000440597534096E-2</v>
+        <v>2.0896501541137602</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B56" s="2">
-        <v>4.44600057601928</v>
+        <v>3.8679993152618399</v>
       </c>
       <c r="C56" s="2">
-        <v>6.9000244140625E-2</v>
+        <v>4.90002632141113E-2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B57" s="2">
-        <v>18.912998676299999</v>
+        <v>4.7180001735687203</v>
       </c>
       <c r="C57" s="2">
-        <v>0.544999599456787</v>
+        <v>7.7999591827392495E-2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B58" s="2">
-        <v>26.490000009536701</v>
+        <v>360.01499962806702</v>
       </c>
       <c r="C58" s="2">
-        <v>0.41500186920165999</v>
+        <v>0.10300064086914</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B59" s="2">
-        <v>5.9689984321594203</v>
+        <v>3.91099905967712</v>
       </c>
       <c r="C59" s="2">
-        <v>0.183001518249511</v>
+        <v>4.80005741119384E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B60" s="2">
-        <v>85.954000473022404</v>
+        <v>8.6899998188018799</v>
       </c>
       <c r="C60" s="2">
-        <v>4.0629978179931596</v>
+        <v>0.111000299453735</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B61" s="2">
-        <v>4.0339996814727703</v>
+        <v>24.801000356674098</v>
       </c>
       <c r="C61" s="2">
-        <v>0.19999957084655701</v>
+        <v>0.35900020599365201</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B62" s="2">
-        <v>17.325000047683702</v>
+        <v>9.3379995822906494</v>
       </c>
       <c r="C62" s="2">
-        <v>0.14899849891662501</v>
+        <v>9.0001821517944294E-2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B63" s="2">
-        <v>22.0539999008178</v>
+        <v>37.342998027801499</v>
       </c>
       <c r="C63" s="2">
-        <v>0.188999652862548</v>
+        <v>0.28899908065795898</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B64" s="2">
-        <v>7.3510003089904696</v>
+        <v>8.75500035285949</v>
       </c>
       <c r="C64" s="2">
-        <v>0.24599981307983301</v>
+        <v>0.12700200080871499</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B65" s="2">
-        <v>44.3009994029998</v>
+        <v>7.9739995002746502</v>
       </c>
       <c r="C65" s="2">
-        <v>0.41399908065795898</v>
+        <v>0.12499952316284101</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B66" s="2">
-        <v>3.8640003204345699</v>
+        <v>6.3209996223449698</v>
       </c>
       <c r="C66" s="2">
-        <v>0.105998754501342</v>
+        <v>6.3000440597534096E-2</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B67" s="2">
-        <v>28.367000579833899</v>
+        <v>4.44600057601928</v>
       </c>
       <c r="C67" s="2">
-        <v>0.445999145507812</v>
+        <v>6.9000244140625E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B68" s="2">
-        <v>9.8130009174346906</v>
+        <v>18.912998676299999</v>
       </c>
       <c r="C68" s="2">
-        <v>0.16200065612792899</v>
+        <v>0.544999599456787</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B69" s="2">
-        <v>9.2119987010955793</v>
+        <v>26.490000009536701</v>
       </c>
       <c r="C69" s="2">
-        <v>9.3000173568725503E-2</v>
+        <v>0.41500186920165999</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B70" s="2">
-        <v>26.832000255584699</v>
+        <v>5.9689984321594203</v>
       </c>
       <c r="C70" s="2">
-        <v>1.85600090026855</v>
+        <v>0.183001518249511</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B71" s="2">
-        <v>4.8450002670287997</v>
+        <v>85.954000473022404</v>
       </c>
       <c r="C71" s="2">
-        <v>0.18000054359435999</v>
+        <v>4.0629978179931596</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B72" s="2">
-        <v>11.4260003566741</v>
+        <v>4.0339996814727703</v>
       </c>
       <c r="C72" s="2">
-        <v>0.32800054550170898</v>
+        <v>0.19999957084655701</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B73" s="2">
-        <v>19.375999450683501</v>
+        <v>17.325000047683702</v>
       </c>
       <c r="C73" s="2">
-        <v>8.0000877380371094E-2</v>
+        <v>0.14899849891662501</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B74" s="2">
-        <v>1.16900038719177</v>
+        <v>22.0539999008178</v>
       </c>
       <c r="C74" s="2">
-        <v>8.8999748229980399E-2</v>
+        <v>0.188999652862548</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B75" s="2">
-        <v>0.92900013923644997</v>
+        <v>7.3510003089904696</v>
       </c>
       <c r="C75" s="2">
-        <v>9.9000692367553697E-2</v>
+        <v>0.24599981307983301</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B76" s="2">
-        <v>5.1230006217956499</v>
+        <v>44.3009994029998</v>
       </c>
       <c r="C76" s="2">
-        <v>0.124008178710937</v>
+        <v>0.41399908065795898</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B77" s="2">
-        <v>4.7509996891021702</v>
+        <v>3.8640003204345699</v>
       </c>
       <c r="C77" s="2">
-        <v>0.120999097824096</v>
+        <v>0.105998754501342</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B78" s="2">
-        <v>47.340000391006399</v>
+        <v>360.00800037383999</v>
       </c>
       <c r="C78" s="2">
-        <v>0.37900972366333002</v>
+        <v>0.84200024604797297</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B79" s="2">
-        <v>32.6019992828369</v>
+        <v>28.367000579833899</v>
       </c>
       <c r="C79" s="2">
-        <v>0.35899972915649397</v>
+        <v>0.445999145507812</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B80" s="2">
-        <v>6.4560000896453804</v>
+        <v>9.8130009174346906</v>
       </c>
       <c r="C80" s="2">
-        <v>0.164000034332275</v>
+        <v>0.16200065612792899</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B81" s="2">
-        <v>2.8880014419555602</v>
+        <v>9.2119987010955793</v>
       </c>
       <c r="C81" s="2">
-        <v>2.6999473571777299E-2</v>
+        <v>9.3000173568725503E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B82" s="2">
-        <v>0.73499846458435003</v>
+        <v>26.832000255584699</v>
       </c>
       <c r="C82" s="2">
-        <v>3.5999298095703097E-2</v>
+        <v>1.85600090026855</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B83" s="2">
-        <v>148.50999927520701</v>
+        <v>4.8450002670287997</v>
       </c>
       <c r="C83" s="2">
-        <v>4.6998977661132799E-2</v>
+        <v>0.18000054359435999</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B84" s="2">
-        <v>7.95900130271911</v>
+        <v>11.4260003566741</v>
       </c>
       <c r="C84" s="2">
-        <v>0.274999380111694</v>
+        <v>0.32800054550170898</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B85" s="2">
-        <v>4.5410003662109304</v>
+        <v>360.01600003242402</v>
       </c>
       <c r="C85" s="2">
-        <v>3.4998893737792899E-2</v>
+        <v>0.26199913024902299</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B86" s="2">
-        <v>14.308999538421601</v>
+        <v>19.375999450683501</v>
       </c>
       <c r="C86" s="2">
-        <v>0.38099908828735302</v>
+        <v>8.0000877380371094E-2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B87" s="2">
-        <v>5.2159998416900599</v>
+        <v>1.16900038719177</v>
       </c>
       <c r="C87" s="2">
-        <v>0.49399995803833002</v>
+        <v>8.8999748229980399E-2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
+        <v>84</v>
+      </c>
+      <c r="B88" s="2">
+        <v>0.92900013923644997</v>
+      </c>
+      <c r="C88" s="2">
+        <v>9.9000692367553697E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="3">
+        <v>85</v>
+      </c>
+      <c r="B89" s="2">
+        <v>5.1230006217956499</v>
+      </c>
+      <c r="C89" s="2">
+        <v>0.124008178710937</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="3">
+        <v>86</v>
+      </c>
+      <c r="B90" s="2">
+        <v>4.7509996891021702</v>
+      </c>
+      <c r="C90" s="2">
+        <v>0.120999097824096</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="3">
+        <v>87</v>
+      </c>
+      <c r="B91" s="2">
+        <v>47.340000391006399</v>
+      </c>
+      <c r="C91" s="2">
+        <v>0.37900972366333002</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="3">
+        <v>88</v>
+      </c>
+      <c r="B92" s="2">
+        <v>32.6019992828369</v>
+      </c>
+      <c r="C92" s="2">
+        <v>0.35899972915649397</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="3">
+        <v>89</v>
+      </c>
+      <c r="B93" s="2">
+        <v>6.4560000896453804</v>
+      </c>
+      <c r="C93" s="2">
+        <v>0.164000034332275</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="3">
+        <v>90</v>
+      </c>
+      <c r="B94" s="2">
+        <v>2.8880014419555602</v>
+      </c>
+      <c r="C94" s="2">
+        <v>2.6999473571777299E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="3">
+        <v>91</v>
+      </c>
+      <c r="B95" s="2">
+        <v>0.73499846458435003</v>
+      </c>
+      <c r="C95" s="2">
+        <v>3.5999298095703097E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="3">
+        <v>92</v>
+      </c>
+      <c r="B96" s="2">
+        <v>148.50999927520701</v>
+      </c>
+      <c r="C96" s="2">
+        <v>4.6998977661132799E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="3">
+        <v>93</v>
+      </c>
+      <c r="B97" s="2">
+        <v>7.95900130271911</v>
+      </c>
+      <c r="C97" s="2">
+        <v>0.274999380111694</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="3">
+        <v>94</v>
+      </c>
+      <c r="B98" s="2">
+        <v>360.00699996948202</v>
+      </c>
+      <c r="C98" s="2">
+        <v>8.8999032974243095E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="3">
+        <v>95</v>
+      </c>
+      <c r="B99" s="2">
+        <v>360.01399993896399</v>
+      </c>
+      <c r="C99" s="2">
+        <v>0.72999811172485296</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="3">
+        <v>96</v>
+      </c>
+      <c r="B100" s="2">
+        <v>4.5410003662109304</v>
+      </c>
+      <c r="C100" s="2">
+        <v>3.4998893737792899E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="3">
+        <v>97</v>
+      </c>
+      <c r="B101" s="2">
+        <v>14.308999538421601</v>
+      </c>
+      <c r="C101" s="2">
+        <v>0.38099908828735302</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="3">
+        <v>98</v>
+      </c>
+      <c r="B102" s="2">
+        <v>5.2159998416900599</v>
+      </c>
+      <c r="C102" s="2">
+        <v>0.49399995803833002</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="3">
         <v>99</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B103" s="2">
         <v>14.206000328063899</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C103" s="2">
         <v>9.8998308181762695E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="3" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B89" s="2">
-        <v>1945.1280071735353</v>
-      </c>
-      <c r="C89" s="2">
-        <v>24.161666870117156</v>
+      <c r="B105" s="2">
+        <v>7345.3060066699909</v>
+      </c>
+      <c r="C105" s="2">
+        <v>31.007657766342113</v>
       </c>
     </row>
   </sheetData>
@@ -22821,4 +23283,1384 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="B2:O35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.6640625" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="9">
+        <v>9.6998691558837793E-2</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="G3" s="7">
+        <v>34</v>
+      </c>
+      <c r="H3" s="9">
+        <v>4.2319991588592503</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0.10099983215331999</v>
+      </c>
+      <c r="J3" s="10">
+        <f>H3/I3</f>
+        <v>41.901051404075417</v>
+      </c>
+      <c r="L3" s="7">
+        <v>67</v>
+      </c>
+      <c r="M3" s="9">
+        <v>85.954000473022404</v>
+      </c>
+      <c r="N3" s="9">
+        <v>4.0629978179931596</v>
+      </c>
+      <c r="O3" s="10">
+        <f>M3/N3</f>
+        <v>21.155315440331137</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3.7479987144470202</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.14099931716918901</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" ref="E4:E35" si="0">C4/D4</f>
+        <v>26.581679895298301</v>
+      </c>
+      <c r="G4" s="7">
+        <v>35</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.304999589920043</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="L4" s="7">
+        <v>68</v>
+      </c>
+      <c r="M4" s="9">
+        <v>4.0339996814727703</v>
+      </c>
+      <c r="N4" s="9">
+        <v>0.19999957084655701</v>
+      </c>
+      <c r="O4" s="10">
+        <f>M4/N4</f>
+        <v>20.170041687578028</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B5" s="7">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>6.8910002708434996</v>
+      </c>
+      <c r="D5" s="9">
+        <v>8.2010269165038993E-2</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" si="0"/>
+        <v>84.026065772030606</v>
+      </c>
+      <c r="G5" s="7">
+        <v>36</v>
+      </c>
+      <c r="H5" s="9">
+        <v>8.7909998893737793</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0.25000166893005299</v>
+      </c>
+      <c r="J5" s="10">
+        <f>H5/I5</f>
+        <v>35.163764814039617</v>
+      </c>
+      <c r="L5" s="7">
+        <v>69</v>
+      </c>
+      <c r="M5" s="9">
+        <v>17.325000047683702</v>
+      </c>
+      <c r="N5" s="9">
+        <v>0.14899849891662501</v>
+      </c>
+      <c r="O5" s="10">
+        <f>M5/N5</f>
+        <v>116.27633951787824</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B6" s="7">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1.58899998664855</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="G6" s="7">
+        <v>37</v>
+      </c>
+      <c r="H6" s="9">
+        <v>18.749999046325598</v>
+      </c>
+      <c r="I6" s="9">
+        <v>4.2999744415283203E-2</v>
+      </c>
+      <c r="J6" s="10">
+        <f>H6/I6</f>
+        <v>436.04908125131487</v>
+      </c>
+      <c r="L6" s="7">
+        <v>70</v>
+      </c>
+      <c r="M6" s="9">
+        <v>22.0539999008178</v>
+      </c>
+      <c r="N6" s="9">
+        <v>0.188999652862548</v>
+      </c>
+      <c r="O6" s="10">
+        <f>M6/N6</f>
+        <v>116.68804448469969</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B7" s="7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8">
+        <v>4.9449999332427899</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.201006174087524</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="0"/>
+        <v>24.601234045127349</v>
+      </c>
+      <c r="G7" s="7">
+        <v>38</v>
+      </c>
+      <c r="H7" s="9">
+        <v>45.683999538421602</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0.26200151443481401</v>
+      </c>
+      <c r="J7" s="10">
+        <f>H7/I7</f>
+        <v>174.36540257017401</v>
+      </c>
+      <c r="L7" s="7">
+        <v>71</v>
+      </c>
+      <c r="M7" s="9">
+        <v>7.3510003089904696</v>
+      </c>
+      <c r="N7" s="9">
+        <v>0.24599981307983301</v>
+      </c>
+      <c r="O7" s="10">
+        <f>M7/N7</f>
+        <v>29.882137782783147</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
+        <v>6</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.16199874877929599</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="G8" s="7">
+        <v>39</v>
+      </c>
+      <c r="H8" s="9">
+        <v>108.573999881744</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0.279998779296875</v>
+      </c>
+      <c r="J8" s="10">
+        <f>H8/I8</f>
+        <v>387.76597581743732</v>
+      </c>
+      <c r="L8" s="7">
+        <v>72</v>
+      </c>
+      <c r="M8" s="9">
+        <v>44.3009994029998</v>
+      </c>
+      <c r="N8" s="9">
+        <v>0.41399908065795898</v>
+      </c>
+      <c r="O8" s="10">
+        <f>M8/N8</f>
+        <v>107.00748255912372</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="7">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8">
+        <v>4.1749997138976997</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.117001056671142</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="0"/>
+        <v>35.683435967868931</v>
+      </c>
+      <c r="G9" s="7">
+        <v>40</v>
+      </c>
+      <c r="H9" s="9">
+        <v>3.12099981307983</v>
+      </c>
+      <c r="I9" s="9">
+        <v>5.5999755859375E-2</v>
+      </c>
+      <c r="J9" s="10">
+        <f>H9/I9</f>
+        <v>55.732382493187941</v>
+      </c>
+      <c r="L9" s="7">
+        <v>73</v>
+      </c>
+      <c r="M9" s="9">
+        <v>3.8640003204345699</v>
+      </c>
+      <c r="N9" s="9">
+        <v>0.105998754501342</v>
+      </c>
+      <c r="O9" s="10">
+        <f>M9/N9</f>
+        <v>36.453261537008437</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="7">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1.3580005168914699</v>
+      </c>
+      <c r="D10" s="9">
+        <v>6.6998958587646401E-2</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" si="0"/>
+        <v>20.268979481449204</v>
+      </c>
+      <c r="G10" s="7">
+        <v>41</v>
+      </c>
+      <c r="H10" s="9">
+        <v>33.771999835968003</v>
+      </c>
+      <c r="I10" s="9">
+        <v>3.0999898910522398E-2</v>
+      </c>
+      <c r="J10" s="10">
+        <f>H10/I10</f>
+        <v>1089.4229021019376</v>
+      </c>
+      <c r="L10" s="7">
+        <v>74</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="N10" s="9">
+        <v>0.84200024604797297</v>
+      </c>
+      <c r="O10" s="10"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8">
+        <v>13.4009993076324</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.36900067329406699</v>
+      </c>
+      <c r="E11" s="10">
+        <f t="shared" si="0"/>
+        <v>36.317005028749008</v>
+      </c>
+      <c r="G11" s="7">
+        <v>42</v>
+      </c>
+      <c r="H11" s="9">
+        <v>4.28199911117553</v>
+      </c>
+      <c r="I11" s="9">
+        <v>4.1000127792358398E-2</v>
+      </c>
+      <c r="J11" s="10">
+        <f>H11/I11</f>
+        <v>104.43867718806497</v>
+      </c>
+      <c r="L11" s="7">
+        <v>75</v>
+      </c>
+      <c r="M11" s="9">
+        <v>28.367000579833899</v>
+      </c>
+      <c r="N11" s="9">
+        <v>0.445999145507812</v>
+      </c>
+      <c r="O11" s="10">
+        <f>M11/N11</f>
+        <v>63.603262171131291</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="7">
+        <v>10</v>
+      </c>
+      <c r="C12" s="8">
+        <v>64.7129998207092</v>
+      </c>
+      <c r="D12" s="9">
+        <v>6.7000865936279297E-2</v>
+      </c>
+      <c r="E12" s="10">
+        <f t="shared" si="0"/>
+        <v>965.85318587156837</v>
+      </c>
+      <c r="G12" s="7">
+        <v>43</v>
+      </c>
+      <c r="H12" s="9">
+        <v>8.4480009078979492</v>
+      </c>
+      <c r="I12" s="9">
+        <v>8.9000701904296806E-2</v>
+      </c>
+      <c r="J12" s="10">
+        <f>H12/I12</f>
+        <v>94.920609918134744</v>
+      </c>
+      <c r="L12" s="7">
+        <v>76</v>
+      </c>
+      <c r="M12" s="9">
+        <v>9.8130009174346906</v>
+      </c>
+      <c r="N12" s="9">
+        <v>0.16200065612792899</v>
+      </c>
+      <c r="O12" s="10">
+        <f>M12/N12</f>
+        <v>60.573834402778843</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="7">
+        <v>11</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.98100113868713301</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="G13" s="7">
+        <v>44</v>
+      </c>
+      <c r="H13" s="9">
+        <v>16.201998472213699</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0.118000507354736</v>
+      </c>
+      <c r="J13" s="10">
+        <f>H13/I13</f>
+        <v>137.30448144182006</v>
+      </c>
+      <c r="L13" s="7">
+        <v>77</v>
+      </c>
+      <c r="M13" s="9">
+        <v>9.2119987010955793</v>
+      </c>
+      <c r="N13" s="9">
+        <v>9.3000173568725503E-2</v>
+      </c>
+      <c r="O13" s="10">
+        <f>M13/N13</f>
+        <v>99.053564607468971</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="7">
+        <v>12</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.53599858283996504</v>
+      </c>
+      <c r="D14" s="9">
+        <v>4.2001962661743102E-2</v>
+      </c>
+      <c r="E14" s="10">
+        <f t="shared" si="0"/>
+        <v>12.761274685103508</v>
+      </c>
+      <c r="G14" s="7">
+        <v>45</v>
+      </c>
+      <c r="H14" s="9">
+        <v>1.50599932670593</v>
+      </c>
+      <c r="I14" s="9">
+        <v>9.4999790191650293E-2</v>
+      </c>
+      <c r="J14" s="10">
+        <f>H14/I14</f>
+        <v>15.85265950238167</v>
+      </c>
+      <c r="L14" s="7">
+        <v>78</v>
+      </c>
+      <c r="M14" s="9">
+        <v>26.832000255584699</v>
+      </c>
+      <c r="N14" s="9">
+        <v>1.85600090026855</v>
+      </c>
+      <c r="O14" s="10">
+        <f>M14/N14</f>
+        <v>14.456889676994392</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="7">
+        <v>13</v>
+      </c>
+      <c r="C15" s="8">
+        <v>3.0560004711151101</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.122003316879272</v>
+      </c>
+      <c r="E15" s="10">
+        <f t="shared" si="0"/>
+        <v>25.048503182410734</v>
+      </c>
+      <c r="G15" s="7">
+        <v>46</v>
+      </c>
+      <c r="H15" s="9">
+        <v>6.0770001411437899</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0.16799736022949199</v>
+      </c>
+      <c r="J15" s="10">
+        <f>H15/I15</f>
+        <v>36.173188274162953</v>
+      </c>
+      <c r="L15" s="7">
+        <v>79</v>
+      </c>
+      <c r="M15" s="9">
+        <v>4.8450002670287997</v>
+      </c>
+      <c r="N15" s="9">
+        <v>0.18000054359435999</v>
+      </c>
+      <c r="O15" s="10">
+        <f>M15/N15</f>
+        <v>26.916586862911061</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="7">
+        <v>14</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1.3559980392455999</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="G16" s="7">
+        <v>47</v>
+      </c>
+      <c r="H16" s="9">
+        <v>58.686999082565301</v>
+      </c>
+      <c r="I16" s="9">
+        <v>0.52799963951110795</v>
+      </c>
+      <c r="J16" s="10">
+        <f>H16/I16</f>
+        <v>111.14969536135574</v>
+      </c>
+      <c r="L16" s="7">
+        <v>80</v>
+      </c>
+      <c r="M16" s="9">
+        <v>11.4260003566741</v>
+      </c>
+      <c r="N16" s="9">
+        <v>0.32800054550170898</v>
+      </c>
+      <c r="O16" s="10">
+        <f>M16/N16</f>
+        <v>34.835309005955807</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B17" s="7">
+        <v>15</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1.1760003566741899</v>
+      </c>
+      <c r="D17" s="9">
+        <v>5.1999807357788003E-2</v>
+      </c>
+      <c r="E17" s="10">
+        <f t="shared" si="0"/>
+        <v>22.615475257103245</v>
+      </c>
+      <c r="G17" s="7">
+        <v>48</v>
+      </c>
+      <c r="H17" s="9">
+        <v>12.483999490737901</v>
+      </c>
+      <c r="I17" s="9">
+        <v>0.149005651473999</v>
+      </c>
+      <c r="J17" s="10">
+        <f>H17/I17</f>
+        <v>83.782053682147207</v>
+      </c>
+      <c r="L17" s="7">
+        <v>81</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="N17" s="9">
+        <v>0.26199913024902299</v>
+      </c>
+      <c r="O17" s="10"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B18" s="7">
+        <v>16</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" s="9">
+        <v>3.0999422073364199E-2</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="G18" s="7">
+        <v>49</v>
+      </c>
+      <c r="H18" s="9">
+        <v>17.402998208999598</v>
+      </c>
+      <c r="I18" s="9">
+        <v>0.128981828689575</v>
+      </c>
+      <c r="J18" s="10">
+        <f>H18/I18</f>
+        <v>134.92596891988555</v>
+      </c>
+      <c r="L18" s="7">
+        <v>82</v>
+      </c>
+      <c r="M18" s="9">
+        <v>19.375999450683501</v>
+      </c>
+      <c r="N18" s="9">
+        <v>8.0000877380371094E-2</v>
+      </c>
+      <c r="O18" s="10">
+        <f>M18/N18</f>
+        <v>242.19733689367726</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B19" s="7">
+        <v>17</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D19" s="9">
+        <v>9.8999977111816406E-2</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="G19" s="7">
+        <v>50</v>
+      </c>
+      <c r="H19" s="9">
+        <v>8.0669999122619593</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0.17499876022338801</v>
+      </c>
+      <c r="J19" s="10">
+        <f>H19/I19</f>
+        <v>46.097468930433209</v>
+      </c>
+      <c r="L19" s="7">
+        <v>83</v>
+      </c>
+      <c r="M19" s="9">
+        <v>1.16900038719177</v>
+      </c>
+      <c r="N19" s="9">
+        <v>8.8999748229980399E-2</v>
+      </c>
+      <c r="O19" s="10">
+        <f>M19/N19</f>
+        <v>13.134872968078591</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B20" s="7">
+        <v>18</v>
+      </c>
+      <c r="C20" s="8">
+        <v>4.0940003395080504</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.189991950988769</v>
+      </c>
+      <c r="E20" s="10">
+        <f t="shared" si="0"/>
+        <v>21.548283062528576</v>
+      </c>
+      <c r="G20" s="7">
+        <v>51</v>
+      </c>
+      <c r="H20" s="9">
+        <v>33.3270003795623</v>
+      </c>
+      <c r="I20" s="9">
+        <v>2.0896501541137602</v>
+      </c>
+      <c r="J20" s="10">
+        <f>H20/I20</f>
+        <v>15.9486028385917</v>
+      </c>
+      <c r="L20" s="7">
+        <v>84</v>
+      </c>
+      <c r="M20" s="9">
+        <v>0.92900013923644997</v>
+      </c>
+      <c r="N20" s="9">
+        <v>9.9000692367553697E-2</v>
+      </c>
+      <c r="O20" s="10">
+        <f>M20/N20</f>
+        <v>9.3837741637948255</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B21" s="7">
+        <v>19</v>
+      </c>
+      <c r="C21" s="8">
+        <v>3.2709991931915199</v>
+      </c>
+      <c r="D21" s="9">
+        <v>7.3999404907226493E-2</v>
+      </c>
+      <c r="E21" s="10">
+        <f t="shared" si="0"/>
+        <v>44.203047271696192</v>
+      </c>
+      <c r="G21" s="7">
+        <v>52</v>
+      </c>
+      <c r="H21" s="9">
+        <v>3.8679993152618399</v>
+      </c>
+      <c r="I21" s="9">
+        <v>4.90002632141113E-2</v>
+      </c>
+      <c r="J21" s="10">
+        <f>H21/I21</f>
+        <v>78.938337501581373</v>
+      </c>
+      <c r="L21" s="7">
+        <v>85</v>
+      </c>
+      <c r="M21" s="9">
+        <v>5.1230006217956499</v>
+      </c>
+      <c r="N21" s="9">
+        <v>0.124008178710937</v>
+      </c>
+      <c r="O21" s="10">
+        <f>M21/N21</f>
+        <v>41.311796327058083</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="7">
+        <v>20</v>
+      </c>
+      <c r="C22" s="8">
+        <v>2.2240002155303902</v>
+      </c>
+      <c r="D22" s="9">
+        <v>5.2999973297119099E-2</v>
+      </c>
+      <c r="E22" s="10">
+        <f t="shared" si="0"/>
+        <v>41.962289359328402</v>
+      </c>
+      <c r="G22" s="7">
+        <v>53</v>
+      </c>
+      <c r="H22" s="9">
+        <v>4.7180001735687203</v>
+      </c>
+      <c r="I22" s="9">
+        <v>7.7999591827392495E-2</v>
+      </c>
+      <c r="J22" s="10">
+        <f>H22/I22</f>
+        <v>60.487498242417942</v>
+      </c>
+      <c r="L22" s="7">
+        <v>86</v>
+      </c>
+      <c r="M22" s="9">
+        <v>4.7509996891021702</v>
+      </c>
+      <c r="N22" s="9">
+        <v>0.120999097824096</v>
+      </c>
+      <c r="O22" s="10">
+        <f>M22/N22</f>
+        <v>39.264752998481008</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B23" s="7">
+        <v>21</v>
+      </c>
+      <c r="C23" s="8">
+        <v>10.644999980926499</v>
+      </c>
+      <c r="D23" s="9">
+        <v>3.7000179290771401E-2</v>
+      </c>
+      <c r="E23" s="10">
+        <f t="shared" si="0"/>
+        <v>287.70130807397408</v>
+      </c>
+      <c r="G23" s="7">
+        <v>54</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0.10300064086914</v>
+      </c>
+      <c r="J23" s="10"/>
+      <c r="L23" s="7">
+        <v>87</v>
+      </c>
+      <c r="M23" s="9">
+        <v>47.340000391006399</v>
+      </c>
+      <c r="N23" s="9">
+        <v>0.37900972366333002</v>
+      </c>
+      <c r="O23" s="10">
+        <f>M23/N23</f>
+        <v>124.90444818523436</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B24" s="7">
+        <v>22</v>
+      </c>
+      <c r="C24" s="8">
+        <v>158.01899957656801</v>
+      </c>
+      <c r="D24" s="9">
+        <v>1.8379993438720701</v>
+      </c>
+      <c r="E24" s="10">
+        <f t="shared" si="0"/>
+        <v>85.973371047931437</v>
+      </c>
+      <c r="G24" s="7">
+        <v>55</v>
+      </c>
+      <c r="H24" s="9">
+        <v>3.91099905967712</v>
+      </c>
+      <c r="I24" s="9">
+        <v>4.80005741119384E-2</v>
+      </c>
+      <c r="J24" s="10">
+        <f>H24/I24</f>
+        <v>81.478172543448835</v>
+      </c>
+      <c r="L24" s="7">
+        <v>88</v>
+      </c>
+      <c r="M24" s="9">
+        <v>32.6019992828369</v>
+      </c>
+      <c r="N24" s="9">
+        <v>0.35899972915649397</v>
+      </c>
+      <c r="O24" s="10">
+        <f>M24/N24</f>
+        <v>90.813436989043367</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B25" s="7">
+        <v>23</v>
+      </c>
+      <c r="C25" s="8">
+        <v>156.75899815559299</v>
+      </c>
+      <c r="D25" s="9">
+        <v>1.11200022697448</v>
+      </c>
+      <c r="E25" s="10">
+        <f t="shared" si="0"/>
+        <v>140.97029330839385</v>
+      </c>
+      <c r="G25" s="7">
+        <v>56</v>
+      </c>
+      <c r="H25" s="9">
+        <v>8.6899998188018799</v>
+      </c>
+      <c r="I25" s="9">
+        <v>0.111000299453735</v>
+      </c>
+      <c r="J25" s="10">
+        <f>H25/I25</f>
+        <v>78.288075451759269</v>
+      </c>
+      <c r="L25" s="7">
+        <v>89</v>
+      </c>
+      <c r="M25" s="9">
+        <v>6.4560000896453804</v>
+      </c>
+      <c r="N25" s="9">
+        <v>0.164000034332275</v>
+      </c>
+      <c r="O25" s="10">
+        <f>M25/N25</f>
+        <v>39.365845964184949</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B26" s="7">
+        <v>24</v>
+      </c>
+      <c r="C26" s="8">
+        <v>5.4300007820129297</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0.170999765396118</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" si="0"/>
+        <v>31.754434103663399</v>
+      </c>
+      <c r="G26" s="7">
+        <v>57</v>
+      </c>
+      <c r="H26" s="9">
+        <v>24.801000356674098</v>
+      </c>
+      <c r="I26" s="9">
+        <v>0.35900020599365201</v>
+      </c>
+      <c r="J26" s="10">
+        <f>H26/I26</f>
+        <v>69.083526813108961</v>
+      </c>
+      <c r="L26" s="7">
+        <v>90</v>
+      </c>
+      <c r="M26" s="9">
+        <v>2.8880014419555602</v>
+      </c>
+      <c r="N26" s="9">
+        <v>2.6999473571777299E-2</v>
+      </c>
+      <c r="O26" s="10">
+        <f>M26/N26</f>
+        <v>106.96510190385358</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B27" s="7">
+        <v>25</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" s="9">
+        <v>7.6998233795166002E-2</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="G27" s="7">
+        <v>58</v>
+      </c>
+      <c r="H27" s="9">
+        <v>9.3379995822906494</v>
+      </c>
+      <c r="I27" s="9">
+        <v>9.0001821517944294E-2</v>
+      </c>
+      <c r="J27" s="10">
+        <f>H27/I27</f>
+        <v>103.75345103908666</v>
+      </c>
+      <c r="L27" s="7">
+        <v>91</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0.73499846458435003</v>
+      </c>
+      <c r="N27" s="9">
+        <v>3.5999298095703097E-2</v>
+      </c>
+      <c r="O27" s="10">
+        <f>M27/N27</f>
+        <v>20.41702209388577</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B28" s="7">
+        <v>26</v>
+      </c>
+      <c r="C28" s="8">
+        <v>4.0800004005432102</v>
+      </c>
+      <c r="D28" s="9">
+        <v>9.6001386642455999E-2</v>
+      </c>
+      <c r="E28" s="10">
+        <f t="shared" si="0"/>
+        <v>42.499390302961061</v>
+      </c>
+      <c r="G28" s="7">
+        <v>59</v>
+      </c>
+      <c r="H28" s="9">
+        <v>37.342998027801499</v>
+      </c>
+      <c r="I28" s="9">
+        <v>0.28899908065795898</v>
+      </c>
+      <c r="J28" s="10">
+        <f>H28/I28</f>
+        <v>129.21493709524393</v>
+      </c>
+      <c r="L28" s="7">
+        <v>92</v>
+      </c>
+      <c r="M28" s="9">
+        <v>148.50999927520701</v>
+      </c>
+      <c r="N28" s="9">
+        <v>4.6998977661132799E-2</v>
+      </c>
+      <c r="O28" s="10">
+        <f>M28/N28</f>
+        <v>3159.8559514629987</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B29" s="7">
+        <v>27</v>
+      </c>
+      <c r="C29" s="8">
+        <v>4.6739976406097403</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0.25000071525573703</v>
+      </c>
+      <c r="E29" s="10">
+        <f t="shared" si="0"/>
+        <v>18.695937072933958</v>
+      </c>
+      <c r="G29" s="7">
+        <v>60</v>
+      </c>
+      <c r="H29" s="9">
+        <v>8.75500035285949</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0.12700200080871499</v>
+      </c>
+      <c r="J29" s="10">
+        <f>H29/I29</f>
+        <v>68.935924608352423</v>
+      </c>
+      <c r="L29" s="7">
+        <v>93</v>
+      </c>
+      <c r="M29" s="9">
+        <v>7.95900130271911</v>
+      </c>
+      <c r="N29" s="9">
+        <v>0.274999380111694</v>
+      </c>
+      <c r="O29" s="10">
+        <f>M29/N29</f>
+        <v>28.941888158025936</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B30" s="7">
+        <v>28</v>
+      </c>
+      <c r="C30" s="8">
+        <v>28.235001087188699</v>
+      </c>
+      <c r="D30" s="9">
+        <v>0.29500198364257801</v>
+      </c>
+      <c r="E30" s="10">
+        <f t="shared" si="0"/>
+        <v>95.711224509588362</v>
+      </c>
+      <c r="G30" s="7">
+        <v>61</v>
+      </c>
+      <c r="H30" s="9">
+        <v>7.9739995002746502</v>
+      </c>
+      <c r="I30" s="9">
+        <v>0.12499952316284101</v>
+      </c>
+      <c r="J30" s="10">
+        <f>H30/I30</f>
+        <v>63.792239350278621</v>
+      </c>
+      <c r="L30" s="7">
+        <v>94</v>
+      </c>
+      <c r="M30" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="N30" s="9">
+        <v>8.8999032974243095E-2</v>
+      </c>
+      <c r="O30" s="10"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B31" s="7">
+        <v>29</v>
+      </c>
+      <c r="C31" s="8">
+        <v>11.0999996662139</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0.142001867294311</v>
+      </c>
+      <c r="E31" s="10">
+        <f t="shared" si="0"/>
+        <v>78.167983828045038</v>
+      </c>
+      <c r="G31" s="7">
+        <v>62</v>
+      </c>
+      <c r="H31" s="9">
+        <v>6.3209996223449698</v>
+      </c>
+      <c r="I31" s="9">
+        <v>6.3000440597534096E-2</v>
+      </c>
+      <c r="J31" s="10">
+        <f>H31/I31</f>
+        <v>100.33262565138918</v>
+      </c>
+      <c r="L31" s="7">
+        <v>95</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="N31" s="9">
+        <v>0.72999811172485296</v>
+      </c>
+      <c r="O31" s="10"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B32" s="7">
+        <v>30</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.12299990653991601</v>
+      </c>
+      <c r="E32" s="10"/>
+      <c r="G32" s="7">
+        <v>63</v>
+      </c>
+      <c r="H32" s="9">
+        <v>4.44600057601928</v>
+      </c>
+      <c r="I32" s="9">
+        <v>6.9000244140625E-2</v>
+      </c>
+      <c r="J32" s="10">
+        <f>H32/I32</f>
+        <v>64.434562969924713</v>
+      </c>
+      <c r="L32" s="7">
+        <v>96</v>
+      </c>
+      <c r="M32" s="9">
+        <v>4.5410003662109304</v>
+      </c>
+      <c r="N32" s="9">
+        <v>3.4998893737792899E-2</v>
+      </c>
+      <c r="O32" s="10">
+        <f>M32/N32</f>
+        <v>129.74696858225025</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B33" s="7">
+        <v>31</v>
+      </c>
+      <c r="C33" s="8">
+        <v>43.010000705718902</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.16199898719787501</v>
+      </c>
+      <c r="E33" s="10">
+        <f t="shared" si="0"/>
+        <v>265.4954913587452</v>
+      </c>
+      <c r="G33" s="7">
+        <v>64</v>
+      </c>
+      <c r="H33" s="9">
+        <v>18.912998676299999</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0.544999599456787</v>
+      </c>
+      <c r="J33" s="10">
+        <f>H33/I33</f>
+        <v>34.702775369286506</v>
+      </c>
+      <c r="L33" s="7">
+        <v>97</v>
+      </c>
+      <c r="M33" s="9">
+        <v>14.308999538421601</v>
+      </c>
+      <c r="N33" s="9">
+        <v>0.38099908828735302</v>
+      </c>
+      <c r="O33" s="10">
+        <f>M33/N33</f>
+        <v>37.556519105446313</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B34" s="7">
+        <v>32</v>
+      </c>
+      <c r="C34" s="8">
+        <v>250.40202474594099</v>
+      </c>
+      <c r="D34" s="9">
+        <v>1.0999917984008701E-2</v>
+      </c>
+      <c r="E34" s="10">
+        <f t="shared" si="0"/>
+        <v>22763.990159741807</v>
+      </c>
+      <c r="G34" s="7">
+        <v>65</v>
+      </c>
+      <c r="H34" s="9">
+        <v>26.490000009536701</v>
+      </c>
+      <c r="I34" s="9">
+        <v>0.41500186920165999</v>
+      </c>
+      <c r="J34" s="10">
+        <f>H34/I34</f>
+        <v>63.831037822782754</v>
+      </c>
+      <c r="L34" s="7">
+        <v>98</v>
+      </c>
+      <c r="M34" s="9">
+        <v>5.2159998416900599</v>
+      </c>
+      <c r="N34" s="9">
+        <v>0.49399995803833002</v>
+      </c>
+      <c r="O34" s="10">
+        <f>M34/N34</f>
+        <v>10.558705029860235</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B35" s="7">
+        <v>33</v>
+      </c>
+      <c r="C35" s="8">
+        <v>6.7539994716644198</v>
+      </c>
+      <c r="D35" s="9">
+        <v>7.3999404907226493E-2</v>
+      </c>
+      <c r="E35" s="10">
+        <f t="shared" si="0"/>
+        <v>91.270997113178822</v>
+      </c>
+      <c r="G35" s="7">
+        <v>66</v>
+      </c>
+      <c r="H35" s="9">
+        <v>5.9689984321594203</v>
+      </c>
+      <c r="I35" s="9">
+        <v>0.183001518249511</v>
+      </c>
+      <c r="J35" s="10">
+        <f t="shared" ref="J35:J68" si="1">H35/I35</f>
+        <v>32.617207164484114</v>
+      </c>
+      <c r="L35" s="7">
+        <v>99</v>
+      </c>
+      <c r="M35" s="9">
+        <v>14.206000328063899</v>
+      </c>
+      <c r="N35" s="9">
+        <v>9.8998308181762695E-2</v>
+      </c>
+      <c r="O35" s="10">
+        <f>M35/N35</f>
+        <v>143.49740504637134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>